<commit_message>
added code and data
</commit_message>
<xml_diff>
--- a/Coursera-Applied Plotting, Charting & Data Representation in Python (Final Assignment)/ann_arbor.xlsx
+++ b/Coursera-Applied Plotting, Charting & Data Representation in Python (Final Assignment)/ann_arbor.xlsx
@@ -22,18 +22,23 @@
     <t>Growth</t>
   </si>
   <si>
-    <t>Annual Growth Rate</t>
+    <t>Growth Rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;Open Sans&quot;"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -60,7 +65,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -77,6 +82,18 @@
       <alignment horizontal="left" readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -320,13 +337,13 @@
         <v>2021.0</v>
       </c>
       <c r="B2" s="3">
-        <v>117082.0</v>
+        <v>363837.0</v>
       </c>
       <c r="C2" s="3">
-        <v>-1449.0</v>
+        <v>-1882.0</v>
       </c>
       <c r="D2" s="4">
-        <v>-0.0122</v>
+        <v>-0.0052</v>
       </c>
     </row>
     <row r="3">
@@ -334,13 +351,13 @@
         <v>2020.0</v>
       </c>
       <c r="B3" s="3">
-        <v>118531.0</v>
+        <v>365719.0</v>
       </c>
       <c r="C3" s="3">
-        <v>-1449.0</v>
+        <v>-1882.0</v>
       </c>
       <c r="D3" s="4">
-        <v>-0.0121</v>
+        <v>-0.0051</v>
       </c>
     </row>
     <row r="4">
@@ -348,13 +365,13 @@
         <v>2019.0</v>
       </c>
       <c r="B4" s="3">
-        <v>119980.0</v>
+        <v>367601.0</v>
       </c>
       <c r="C4" s="3">
-        <v>-1449.0</v>
+        <v>-1882.0</v>
       </c>
       <c r="D4" s="4">
-        <v>-0.0119</v>
+        <v>-0.0051</v>
       </c>
     </row>
     <row r="5">
@@ -362,13 +379,13 @@
         <v>2018.0</v>
       </c>
       <c r="B5" s="3">
-        <v>121429.0</v>
+        <v>369483.0</v>
       </c>
       <c r="C5" s="2">
-        <v>-64.0</v>
+        <v>676.0</v>
       </c>
       <c r="D5" s="4">
-        <v>-5.0E-4</v>
+        <v>0.0018</v>
       </c>
     </row>
     <row r="6">
@@ -376,13 +393,13 @@
         <v>2017.0</v>
       </c>
       <c r="B6" s="3">
-        <v>121493.0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>574.0</v>
+        <v>368807.0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2672.0</v>
       </c>
       <c r="D6" s="4">
-        <v>0.0047</v>
+        <v>0.0072</v>
       </c>
     </row>
     <row r="7">
@@ -390,10 +407,10 @@
         <v>2016.0</v>
       </c>
       <c r="B7" s="3">
-        <v>120919.0</v>
+        <v>366135.0</v>
       </c>
       <c r="C7" s="3">
-        <v>1035.0</v>
+        <v>3160.0</v>
       </c>
       <c r="D7" s="4">
         <v>0.0086</v>
@@ -404,13 +421,13 @@
         <v>2015.0</v>
       </c>
       <c r="B8" s="3">
-        <v>119884.0</v>
+        <v>362975.0</v>
       </c>
       <c r="C8" s="3">
-        <v>1168.0</v>
+        <v>2954.0</v>
       </c>
       <c r="D8" s="4">
-        <v>0.0098</v>
+        <v>0.0081</v>
       </c>
     </row>
     <row r="9">
@@ -418,13 +435,13 @@
         <v>2014.0</v>
       </c>
       <c r="B9" s="3">
-        <v>118716.0</v>
+        <v>360021.0</v>
       </c>
       <c r="C9" s="3">
-        <v>1896.0</v>
+        <v>3981.0</v>
       </c>
       <c r="D9" s="4">
-        <v>0.0162</v>
+        <v>0.0111</v>
       </c>
     </row>
     <row r="10">
@@ -432,13 +449,13 @@
         <v>2013.0</v>
       </c>
       <c r="B10" s="3">
-        <v>116820.0</v>
-      </c>
-      <c r="C10" s="2">
-        <v>741.0</v>
+        <v>356040.0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3737.0</v>
       </c>
       <c r="D10" s="4">
-        <v>0.0064</v>
+        <v>0.0105</v>
       </c>
     </row>
     <row r="11">
@@ -446,13 +463,13 @@
         <v>2012.0</v>
       </c>
       <c r="B11" s="3">
-        <v>116079.0</v>
-      </c>
-      <c r="C11" s="2">
-        <v>540.0</v>
+        <v>352303.0</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2550.0</v>
       </c>
       <c r="D11" s="4">
-        <v>0.0047</v>
+        <v>0.0072</v>
       </c>
     </row>
     <row r="12">
@@ -460,13 +477,13 @@
         <v>2011.0</v>
       </c>
       <c r="B12" s="3">
-        <v>115539.0</v>
+        <v>349753.0</v>
       </c>
       <c r="C12" s="3">
-        <v>1366.0</v>
+        <v>4036.0</v>
       </c>
       <c r="D12" s="4">
-        <v>0.012</v>
+        <v>0.0115</v>
       </c>
     </row>
     <row r="13">
@@ -474,222 +491,102 @@
         <v>2010.0</v>
       </c>
       <c r="B13" s="3">
-        <v>114173.0</v>
-      </c>
-      <c r="C13" s="2">
-        <v>149.0</v>
-      </c>
+        <v>345717.0</v>
+      </c>
+      <c r="C13" s="5"/>
       <c r="D13" s="4">
-        <v>1.0E-4</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2">
-        <v>2000.0</v>
-      </c>
-      <c r="B14" s="3">
-        <v>114024.0</v>
-      </c>
-      <c r="C14" s="3">
-        <v>4432.0</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0.004</v>
-      </c>
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="15">
-      <c r="A15" s="2">
-        <v>1990.0</v>
-      </c>
-      <c r="B15" s="3">
-        <v>109592.0</v>
-      </c>
-      <c r="C15" s="3">
-        <v>1623.0</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0.0015</v>
-      </c>
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
     </row>
     <row r="16">
-      <c r="A16" s="2">
-        <v>1980.0</v>
-      </c>
-      <c r="B16" s="3">
-        <v>107969.0</v>
-      </c>
-      <c r="C16" s="3">
-        <v>7934.0</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0.0077</v>
-      </c>
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
     </row>
     <row r="17">
-      <c r="A17" s="2">
-        <v>1970.0</v>
-      </c>
-      <c r="B17" s="3">
-        <v>100035.0</v>
-      </c>
-      <c r="C17" s="3">
-        <v>32695.0</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0.0404</v>
-      </c>
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
     </row>
     <row r="18">
-      <c r="A18" s="2">
-        <v>1960.0</v>
-      </c>
-      <c r="B18" s="3">
-        <v>67340.0</v>
-      </c>
-      <c r="C18" s="3">
-        <v>19089.0</v>
-      </c>
-      <c r="D18" s="4">
-        <v>0.0339</v>
-      </c>
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8"/>
     </row>
     <row r="19">
-      <c r="A19" s="2">
-        <v>1950.0</v>
-      </c>
-      <c r="B19" s="3">
-        <v>48251.0</v>
-      </c>
-      <c r="C19" s="3">
-        <v>18436.0</v>
-      </c>
-      <c r="D19" s="4">
-        <v>0.0493</v>
-      </c>
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
     </row>
     <row r="20">
-      <c r="A20" s="2">
-        <v>1940.0</v>
-      </c>
-      <c r="B20" s="3">
-        <v>29815.0</v>
-      </c>
-      <c r="C20" s="3">
-        <v>2871.0</v>
-      </c>
-      <c r="D20" s="4">
-        <v>0.0102</v>
-      </c>
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="8"/>
     </row>
     <row r="21">
-      <c r="A21" s="2">
-        <v>1930.0</v>
-      </c>
-      <c r="B21" s="3">
-        <v>26944.0</v>
-      </c>
-      <c r="C21" s="3">
-        <v>7428.0</v>
-      </c>
-      <c r="D21" s="4">
-        <v>0.0328</v>
-      </c>
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="8"/>
     </row>
     <row r="22">
-      <c r="A22" s="2">
-        <v>1920.0</v>
-      </c>
-      <c r="B22" s="3">
-        <v>19516.0</v>
-      </c>
-      <c r="C22" s="3">
-        <v>4699.0</v>
-      </c>
-      <c r="D22" s="4">
-        <v>0.0279</v>
-      </c>
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="8"/>
     </row>
     <row r="23">
-      <c r="A23" s="2">
-        <v>1910.0</v>
-      </c>
-      <c r="B23" s="3">
-        <v>14817.0</v>
-      </c>
-      <c r="C23" s="2">
-        <v>308.0</v>
-      </c>
-      <c r="D23" s="4">
-        <v>0.0021</v>
-      </c>
+      <c r="A23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="8"/>
     </row>
     <row r="24">
-      <c r="A24" s="2">
-        <v>1900.0</v>
-      </c>
-      <c r="B24" s="3">
-        <v>14509.0</v>
-      </c>
-      <c r="C24" s="3">
-        <v>5078.0</v>
-      </c>
-      <c r="D24" s="4">
-        <v>0.044</v>
-      </c>
+      <c r="A24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8"/>
     </row>
     <row r="25">
-      <c r="A25" s="2">
-        <v>1890.0</v>
-      </c>
-      <c r="B25" s="3">
-        <v>9431.0</v>
-      </c>
-      <c r="C25" s="3">
-        <v>1370.0</v>
-      </c>
-      <c r="D25" s="4">
-        <v>0.0158</v>
-      </c>
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="8"/>
     </row>
     <row r="26">
-      <c r="A26" s="2">
-        <v>1880.0</v>
-      </c>
-      <c r="B26" s="3">
-        <v>8061.0</v>
-      </c>
-      <c r="C26" s="2">
-        <v>698.0</v>
-      </c>
-      <c r="D26" s="4">
-        <v>0.0091</v>
-      </c>
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="8"/>
     </row>
     <row r="27">
-      <c r="A27" s="2">
-        <v>1870.0</v>
-      </c>
-      <c r="B27" s="3">
-        <v>7363.0</v>
-      </c>
-      <c r="C27" s="3">
-        <v>2266.0</v>
-      </c>
-      <c r="D27" s="4">
-        <v>0.0375</v>
-      </c>
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="8"/>
     </row>
     <row r="28">
-      <c r="A28" s="2">
-        <v>1860.0</v>
-      </c>
-      <c r="B28" s="3">
-        <v>5097.0</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="4">
-        <v>0.0</v>
-      </c>
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="8"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>